<commit_message>
Usuário e Tipo acrescentados
</commit_message>
<xml_diff>
--- a/Modelagens/Físico/hroads-fisico.xlsx
+++ b/Modelagens/Físico/hroads-fisico.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEV\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEV\Desktop\Hroads\ProjetoHroads-Tarde\Modelagens\Físico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48AA4EB2-26C0-47DD-B1C9-35DBC25613F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DDBA26-F5BA-4D9A-8D8E-7E295B7C3E67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{683B4504-55DE-47B0-AD55-A256E092FDE3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>personagem</t>
   </si>
@@ -130,13 +130,64 @@
   </si>
   <si>
     <t>idHabilidade fk</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>idUsuario</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>Saulove</t>
+  </si>
+  <si>
+    <t>NayNay_777</t>
+  </si>
+  <si>
+    <t>Kaukau_power</t>
+  </si>
+  <si>
+    <t>saulo@email.com</t>
+  </si>
+  <si>
+    <t>nay777@email.com</t>
+  </si>
+  <si>
+    <t>kaueramos@email.com</t>
+  </si>
+  <si>
+    <t>idTipoUsuario</t>
+  </si>
+  <si>
+    <t>saulove123</t>
+  </si>
+  <si>
+    <t>escudeiro_suzaninha</t>
+  </si>
+  <si>
+    <t>zennite007</t>
+  </si>
+  <si>
+    <t>tipoUsuario</t>
+  </si>
+  <si>
+    <t>administrador</t>
+  </si>
+  <si>
+    <t>jogador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +198,27 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -207,11 +279,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,8 +396,57 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C70D7F-EFD4-4CF5-B08E-B9D6C24789E8}">
-  <dimension ref="B2:H29"/>
+  <dimension ref="B2:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,20 +772,21 @@
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -777,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
@@ -791,7 +988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E18" s="2" t="s">
         <v>31</v>
       </c>
@@ -799,11 +996,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="13"/>
       <c r="E19" s="2" t="s">
         <v>32</v>
       </c>
@@ -811,7 +1008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>4</v>
       </c>
@@ -819,7 +1016,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="8">
         <v>1</v>
       </c>
@@ -827,47 +1024,114 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="8">
         <v>2</v>
       </c>
       <c r="C22" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="8">
         <v>3</v>
       </c>
       <c r="C23" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="8">
         <v>4</v>
       </c>
       <c r="C24" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="21">
+        <v>1</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="8">
         <v>5</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="21">
+        <v>2</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="8">
         <v>6</v>
       </c>
       <c r="C26" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="18">
+        <v>3</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="8">
         <v>7</v>
       </c>
@@ -875,28 +1139,55 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <v>1</v>
       </c>
       <c r="C28" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <v>4</v>
       </c>
       <c r="C29" s="10">
         <v>2</v>
       </c>
+      <c r="E29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E30" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="8">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E22:I22"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G24" r:id="rId1" xr:uid="{59613447-262B-463D-B744-62B206BB10FE}"/>
+    <hyperlink ref="G25:G26" r:id="rId2" display="saulo@email.com" xr:uid="{0DE2C8D9-17F5-4D46-A6A8-9086B40775C9}"/>
+    <hyperlink ref="G25" r:id="rId3" xr:uid="{F03B1D03-4108-4219-A334-BAB1416CDC85}"/>
+    <hyperlink ref="G26" r:id="rId4" xr:uid="{14E5DE70-21A5-40A7-A931-1AFAE4FAF6C6}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>